<commit_message>
#SSW-2063 Extends Institution Import
</commit_message>
<xml_diff>
--- a/Common/Style/Resource/Template/Import_Schulen.xlsx
+++ b/Common/Style/Resource/Template/Import_Schulen.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\kundwzwickau.de\kuw\abteilung_software\Projekte\Schulsoftware\30 Projektrealisierung\30.2 Einstieg und Schulung\!Datenimport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA673AF1-9CFD-4CBB-AF14-88F2CB66B69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D17B540-079D-473C-8496-06A1499243CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$P$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$Q$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Optional</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Pflicht</t>
+  </si>
+  <si>
+    <t>Fax_Geschäftlich</t>
   </si>
 </sst>
 </file>
@@ -149,9 +152,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,13 +461,14 @@
     <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -489,8 +493,9 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -531,18 +536,21 @@
         <v>14</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+6JOVhvsy7g0282yQ7PxqlWco98lnkMGkn8l1wnII/I1tO7lBAEas/efx/eVeEGvH0DqemSbnaZS4GWkq9oC+Q==" saltValue="v4W6xwRej0zmlc/ValEycA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A2:P2" xr:uid="{82C49C8B-5DA9-450E-A053-7FBA04DF3CE4}"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="afg4jG8RDt+PCX8EyEEBVFeLaYE3bkVnl1S8PWC7+jXyf9O85UaIf5qFl9zK1wjEU8aDUjYgCyTa4pOKEnhRIw==" saltValue="w76GNC4ep9fz2kDQawQgQA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <autoFilter ref="A2:Q2" xr:uid="{82C49C8B-5DA9-450E-A053-7FBA04DF3CE4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>